<commit_message>
Add minor formatting fixes
</commit_message>
<xml_diff>
--- a/energy_data/xlsx_data/KDI_production_data.xlsx
+++ b/energy_data/xlsx_data/KDI_production_data.xlsx
@@ -199,18 +199,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -221,6 +209,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -239,14 +239,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:K7" totalsRowShown="0">
   <autoFilter ref="A2:K7"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" name="Country" dataDxfId="2"/>
-    <tableColumn id="3" name="Commodity" dataDxfId="0"/>
-    <tableColumn id="4" name="price" dataDxfId="1"/>
-    <tableColumn id="5" name="units" dataDxfId="7"/>
-    <tableColumn id="6" name="quantity" dataDxfId="6"/>
-    <tableColumn id="7" name="units2" dataDxfId="5"/>
-    <tableColumn id="8" name="year" dataDxfId="4"/>
+    <tableColumn id="1" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" name="Country" dataDxfId="6"/>
+    <tableColumn id="3" name="Commodity" dataDxfId="5"/>
+    <tableColumn id="4" name="price" dataDxfId="4"/>
+    <tableColumn id="5" name="units" dataDxfId="3"/>
+    <tableColumn id="6" name="quantity" dataDxfId="2"/>
+    <tableColumn id="7" name="units2" dataDxfId="1"/>
+    <tableColumn id="8" name="year" dataDxfId="0"/>
     <tableColumn id="9" name="Notes"/>
     <tableColumn id="10" name="FULL CITATION"/>
     <tableColumn id="11" name="AUTHOR"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,8 +723,8 @@
         <v>14</v>
       </c>
       <c r="F7" s="4">
-        <f>76570*1000*42*3.78</f>
-        <v>12156253200</v>
+        <f>76570*1000*42</f>
+        <v>3215940000</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>23</v>

</xml_diff>